<commit_message>
Fix filtering issues and implement browser navigation
- Fixed province, city, and area filters not persisting selections
- Implemented proper browser history navigation with URL parameters
- Enhanced back navigation from property details to filtered property list
- Added smart filter restoration from URL, navigation state, or localStorage
- Updated Excel data import functionality for PostgreSQL
- Improved filter cascade logic to only clear invalid selections
</commit_message>
<xml_diff>
--- a/property_research_sample.xlsx
+++ b/property_research_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amoge\Digital Estate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78093342-018E-45AB-ABAB-21237FCA6646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E87278A-88C1-4B0A-8E61-92C5882E7966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="properties" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="142">
   <si>
     <t>property_id</t>
   </si>
@@ -77,9 +77,6 @@
     <t>54321</t>
   </si>
   <si>
-    <t>10 Rivonia Road</t>
-  </si>
-  <si>
     <t>5 Jean Avenue</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>2196</t>
   </si>
   <si>
-    <t>0157</t>
-  </si>
-  <si>
     <t>Commercial</t>
   </si>
   <si>
@@ -290,9 +284,6 @@
     <t>50 West Street</t>
   </si>
   <si>
-    <t>https://example.com/property6_1.jpg,https://example.com/property6_2.jpg</t>
-  </si>
-  <si>
     <t>76 Main Road</t>
   </si>
   <si>
@@ -305,9 +296,6 @@
     <t>12 Leeuwkop Road</t>
   </si>
   <si>
-    <t>https://example.com/property8_1.jpg</t>
-  </si>
-  <si>
     <t>25 Brooklyn Road</t>
   </si>
   <si>
@@ -335,9 +323,6 @@
     <t>14 Rivonia Road</t>
   </si>
   <si>
-    <t>https://example.com/property12_1.jpg</t>
-  </si>
-  <si>
     <t>45 Jan Smuts Avenue</t>
   </si>
   <si>
@@ -444,13 +429,34 @@
   </si>
   <si>
     <t>https://example.com/property24_1.jpg</t>
+  </si>
+  <si>
+    <t>property_name</t>
+  </si>
+  <si>
+    <t>371 Rivonia Boulevard, Rivonia, Sandton, Rivonia</t>
+  </si>
+  <si>
+    <t>Rivonia Boulevard</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1ZI82xWpEBoOanble_ZPUMTzvjKOjkI60/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1ULsGxwKVCzpHk7cMdpN_nT_spqNvjYHr/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1IG3oJpIL9wSYQj9RC0Zkn3nMAWbeAjcQ/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1rQzxvlt4ESEtbV5vkFzMm9JaFL2zukAc/view?usp=drive_link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -480,6 +486,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF0D63C9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -489,7 +501,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -527,12 +539,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -546,12 +584,540 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFCCCCCC"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFCCCCCC"/>
+        </right>
+        <top style="medium">
+          <color rgb="FFCCCCCC"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -562,6 +1128,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D22670CB-BC3B-4D82-B15C-2A04F0AE5DD4}" name="Table1" displayName="Table1" ref="D1:P25" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="15" tableBorderDxfId="16">
+  <autoFilter ref="D1:P25" xr:uid="{D22670CB-BC3B-4D82-B15C-2A04F0AE5DD4}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{999FD1A3-128A-4F56-88BC-FED56F3EA866}" name="street_address" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{E2A59FC4-0C3E-4E3B-B9E0-C2B01872C1B7}" name="suburb" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{41E8AC58-AEB3-451D-A452-92386CA164E0}" name="city" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{C5343E52-444F-46E3-A3DA-2252D6E73060}" name="province" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{C1B585A9-9BC9-4BAA-B2F6-866C954A683B}" name="postal_code" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{EFE0C017-9450-4F1A-B2CE-B7CA6D35070D}" name="property_type" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{5E71D537-823A-4DA1-A271-F62C673D4455}" name="erf_size_sqm" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{FF958E83-63FF-40A4-A55A-CD0962E657E2}" name="building_size_sqm" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{77A164F5-630F-4413-8ACA-88940F9AFFA3}" name="year_built" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{32DA0702-66A2-4EBB-AA08-DFA8B7CAB599}" name="condition" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{F930F90A-74E3-4691-90C0-CC7559A9BD1A}" name="latitude" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{CE95DC10-837D-4465-98B9-5AE084CDC5F6}" name="longitude" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{3B03EE82-7229-4025-B62A-A58469DC2395}" name="images" dataDxfId="2" dataCellStyle="Hyperlink"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -851,1223 +1439,1258 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="69.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="69.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P1" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
+      <c r="D2" s="5" t="s">
+        <v>136</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>26</v>
       </c>
-      <c r="H2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2">
+      <c r="J2">
         <v>2500</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>1800</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>2010</v>
       </c>
-      <c r="L2" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2">
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2">
         <v>-26.107600000000001</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>28.056699999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2" s="13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" s="6">
+        <v>2194</v>
+      </c>
+      <c r="I3" t="s">
         <v>27</v>
       </c>
-      <c r="H3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3">
+      <c r="J3">
         <v>1200</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>900</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>2015</v>
       </c>
-      <c r="L3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3">
+      <c r="M3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3">
         <v>-25.864999999999998</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>28.1891</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
       <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4">
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4">
         <v>3000</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>2500</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>2008</v>
       </c>
-      <c r="L4" t="s">
-        <v>33</v>
-      </c>
-      <c r="M4">
+      <c r="M4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4">
         <v>-26.145600000000002</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>28.0411</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2">
         <v>98765</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="7">
+        <v>2194</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="2">
+        <v>850</v>
+      </c>
+      <c r="K5" s="2">
+        <v>450</v>
+      </c>
+      <c r="L5" s="2">
+        <v>2005</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" s="2">
+        <v>-26.0823</v>
+      </c>
+      <c r="O5" s="2">
+        <v>27.9712</v>
+      </c>
+      <c r="P5" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="2">
-        <v>2194</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="2">
-        <v>850</v>
-      </c>
-      <c r="J5" s="2">
-        <v>450</v>
-      </c>
-      <c r="K5" s="2">
-        <v>2005</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" s="2">
-        <v>-26.0823</v>
-      </c>
-      <c r="N5" s="2">
-        <v>27.9712</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2">
         <v>11223</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="7">
+        <v>28</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1500</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1200</v>
+      </c>
+      <c r="L6" s="2">
+        <v>2012</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N6" s="2">
+        <v>-25.753299999999999</v>
+      </c>
+      <c r="O6" s="2">
+        <v>28.232299999999999</v>
+      </c>
+      <c r="P6" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="2">
-        <v>28</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="2">
-        <v>1500</v>
-      </c>
-      <c r="J6" s="2">
-        <v>1200</v>
-      </c>
-      <c r="K6" s="2">
-        <v>2012</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="M6" s="2">
-        <v>-25.753299999999999</v>
-      </c>
-      <c r="N6" s="2">
-        <v>28.232299999999999</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2">
         <v>45678</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="2">
+        <v>22</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="7">
         <v>2196</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="2">
+      <c r="I7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="2">
         <v>4000</v>
       </c>
-      <c r="J7" s="2">
+      <c r="K7" s="2">
         <v>3500</v>
       </c>
-      <c r="K7" s="2">
+      <c r="L7" s="2">
         <v>2018</v>
       </c>
-      <c r="L7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M7" s="2">
+      <c r="M7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" s="2">
         <v>-26.104500000000002</v>
       </c>
-      <c r="N7" s="2">
+      <c r="O7" s="2">
         <v>28.051100000000002</v>
       </c>
-      <c r="O7" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P7" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2">
         <v>22334</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>89</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="2">
+        <v>22</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="7">
         <v>2191</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" s="2">
+      <c r="I8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="2">
         <v>1500</v>
       </c>
-      <c r="J8" s="2">
+      <c r="K8" s="2">
         <v>700</v>
       </c>
-      <c r="K8" s="2">
+      <c r="L8" s="2">
         <v>2017</v>
       </c>
-      <c r="L8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M8" s="2">
+      <c r="M8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N8" s="2">
         <v>-26.046700000000001</v>
       </c>
-      <c r="N8" s="2">
+      <c r="O8" s="2">
         <v>28.012499999999999</v>
       </c>
-      <c r="O8" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P8" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2">
         <v>34567</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>92</v>
-      </c>
       <c r="D9" s="3" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="2">
+        <v>22</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="7">
         <v>2157</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" s="2">
+      <c r="I9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="2">
         <v>1050</v>
       </c>
-      <c r="J9" s="2">
+      <c r="K9" s="2">
         <v>550</v>
       </c>
-      <c r="K9" s="2">
+      <c r="L9" s="2">
         <v>2013</v>
       </c>
-      <c r="L9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M9" s="2">
+      <c r="M9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" s="2">
         <v>-26.023399999999999</v>
       </c>
-      <c r="N9" s="2">
+      <c r="O9" s="2">
         <v>28.055599999999998</v>
       </c>
-      <c r="O9" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P9" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2">
         <v>89012</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="2">
+      <c r="H10" s="7">
         <v>181</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="2">
+      <c r="I10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="2">
         <v>1800</v>
       </c>
-      <c r="J10" s="2">
+      <c r="K10" s="2">
         <v>1500</v>
       </c>
-      <c r="K10" s="2">
+      <c r="L10" s="2">
         <v>2005</v>
       </c>
-      <c r="L10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="M10" s="2">
+      <c r="M10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N10" s="2">
         <v>-25.772500000000001</v>
       </c>
-      <c r="N10" s="2">
+      <c r="O10" s="2">
         <v>28.232299999999999</v>
       </c>
-      <c r="O10" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P10" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2">
         <v>10987</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="2">
+        <v>22</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="7">
         <v>2191</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="2">
+        <v>2800</v>
+      </c>
+      <c r="K11" s="2">
+        <v>2200</v>
+      </c>
+      <c r="L11" s="2">
+        <v>2011</v>
+      </c>
+      <c r="M11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="2">
-        <v>2800</v>
-      </c>
-      <c r="J11" s="2">
-        <v>2200</v>
-      </c>
-      <c r="K11" s="2">
-        <v>2011</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M11" s="2">
+      <c r="N11" s="2">
         <v>-26.068899999999999</v>
       </c>
-      <c r="N11" s="2">
+      <c r="O11" s="2">
         <v>28.026700000000002</v>
       </c>
-      <c r="O11" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P11" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2">
         <v>21098</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="D12" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="2">
+      <c r="H12" s="7">
         <v>184</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="I12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="2">
+        <v>950</v>
+      </c>
+      <c r="K12" s="2">
+        <v>480</v>
+      </c>
+      <c r="L12" s="2">
+        <v>2016</v>
+      </c>
+      <c r="M12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="2">
-        <v>950</v>
-      </c>
-      <c r="J12" s="2">
-        <v>480</v>
-      </c>
-      <c r="K12" s="2">
-        <v>2016</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M12" s="2">
+      <c r="N12" s="2">
         <v>-25.753299999999999</v>
       </c>
-      <c r="N12" s="2">
+      <c r="O12" s="2">
         <v>28.271100000000001</v>
       </c>
-      <c r="O12" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P12" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2">
         <v>56789</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="2">
+        <v>22</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="7">
         <v>2128</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="2">
+      <c r="I13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="2">
         <v>2000</v>
       </c>
-      <c r="J13" s="2">
+      <c r="K13" s="2">
         <v>1750</v>
       </c>
-      <c r="K13" s="2">
+      <c r="L13" s="2">
         <v>2019</v>
       </c>
-      <c r="L13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M13" s="2">
+      <c r="M13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N13" s="2">
         <v>-26.059799999999999</v>
       </c>
-      <c r="N13" s="2">
+      <c r="O13" s="2">
         <v>28.062100000000001</v>
       </c>
-      <c r="O13" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P13" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2">
         <v>13579</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>104</v>
-      </c>
       <c r="D14" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>23</v>
+        <v>100</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="2">
+        <v>22</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="7">
         <v>2196</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I14" s="2">
+      <c r="I14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" s="2">
         <v>1300</v>
       </c>
-      <c r="J14" s="2">
+      <c r="K14" s="2">
         <v>650</v>
       </c>
-      <c r="K14" s="2">
+      <c r="L14" s="2">
         <v>2014</v>
       </c>
-      <c r="L14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="M14" s="2">
+      <c r="M14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N14" s="2">
         <v>-26.130099999999999</v>
       </c>
-      <c r="N14" s="2">
+      <c r="O14" s="2">
         <v>28.031500000000001</v>
       </c>
-      <c r="O14" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P14" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2">
         <v>24680</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="D15" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="2">
+      <c r="H15" s="7">
         <v>81</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I15" s="2">
+      <c r="I15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="2">
         <v>2200</v>
       </c>
-      <c r="J15" s="2">
+      <c r="K15" s="2">
         <v>1900</v>
       </c>
-      <c r="K15" s="2">
+      <c r="L15" s="2">
         <v>2009</v>
       </c>
-      <c r="L15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M15" s="2">
+      <c r="M15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N15" s="2">
         <v>-25.7667</v>
       </c>
-      <c r="N15" s="2">
+      <c r="O15" s="2">
         <v>28.261099999999999</v>
       </c>
-      <c r="O15" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P15" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2">
         <v>36912</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>110</v>
-      </c>
       <c r="D16" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>23</v>
+        <v>106</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="2">
+        <v>22</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" s="7">
         <v>2198</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I16" s="2">
+      <c r="I16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J16" s="2">
         <v>1500</v>
       </c>
-      <c r="J16" s="2">
+      <c r="K16" s="2">
         <v>800</v>
       </c>
-      <c r="K16" s="2">
+      <c r="L16" s="2">
         <v>2001</v>
       </c>
-      <c r="L16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M16" s="2">
+      <c r="M16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N16" s="2">
         <v>-26.159199999999998</v>
       </c>
-      <c r="N16" s="2">
+      <c r="O16" s="2">
         <v>28.046299999999999</v>
       </c>
-      <c r="O16" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P16" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2">
         <v>15935</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>23</v>
+        <v>109</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="2">
+        <v>22</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="7">
         <v>2196</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I17" s="2">
+      <c r="I17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" s="2">
         <v>3500</v>
       </c>
-      <c r="J17" s="2">
+      <c r="K17" s="2">
         <v>3000</v>
       </c>
-      <c r="K17" s="2">
+      <c r="L17" s="2">
         <v>2017</v>
       </c>
-      <c r="L17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M17" s="2">
+      <c r="M17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N17" s="2">
         <v>-26.1265</v>
       </c>
-      <c r="N17" s="2">
+      <c r="O17" s="2">
         <v>28.056699999999999</v>
       </c>
-      <c r="O17" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P17" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2">
         <v>24758</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>116</v>
-      </c>
       <c r="D18" s="3" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="2">
+      <c r="H18" s="7">
         <v>43</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I18" s="2">
+      <c r="I18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" s="2">
         <v>750</v>
       </c>
-      <c r="J18" s="2">
+      <c r="K18" s="2">
         <v>350</v>
       </c>
-      <c r="K18" s="2">
+      <c r="L18" s="2">
         <v>2010</v>
       </c>
-      <c r="L18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M18" s="2">
+      <c r="M18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N18" s="2">
         <v>-25.7987</v>
       </c>
-      <c r="N18" s="2">
+      <c r="O18" s="2">
         <v>28.2911</v>
       </c>
-      <c r="O18" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P18" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2">
         <v>36890</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="D19" s="3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>23</v>
+        <v>115</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="2">
+        <v>22</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="7">
         <v>2193</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I19" s="2">
+      <c r="I19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" s="2">
         <v>2800</v>
       </c>
-      <c r="J19" s="2">
+      <c r="K19" s="2">
         <v>2500</v>
       </c>
-      <c r="K19" s="2">
+      <c r="L19" s="2">
         <v>2007</v>
       </c>
-      <c r="L19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M19" s="2">
+      <c r="M19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N19" s="2">
         <v>-26.177800000000001</v>
       </c>
-      <c r="N19" s="2">
+      <c r="O19" s="2">
         <v>28.031500000000001</v>
       </c>
-      <c r="O19" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P19" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2">
         <v>45698</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="D20" s="3" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>23</v>
+        <v>118</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="2">
+        <v>22</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="7">
         <v>2055</v>
       </c>
-      <c r="H20" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I20" s="2">
+      <c r="I20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" s="2">
         <v>1100</v>
       </c>
-      <c r="J20" s="2">
+      <c r="K20" s="2">
         <v>600</v>
       </c>
-      <c r="K20" s="2">
+      <c r="L20" s="2">
         <v>2019</v>
       </c>
-      <c r="L20" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="M20" s="2">
+      <c r="M20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N20" s="2">
         <v>-26.0123</v>
       </c>
-      <c r="N20" s="2">
+      <c r="O20" s="2">
         <v>28.001100000000001</v>
       </c>
-      <c r="O20" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P20" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2">
         <v>54327</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="D21" s="3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21" s="2">
+      <c r="H21" s="7">
         <v>181</v>
       </c>
-      <c r="H21" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I21" s="2">
+      <c r="I21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J21" s="2">
         <v>4500</v>
       </c>
-      <c r="J21" s="2">
+      <c r="K21" s="2">
         <v>4000</v>
       </c>
-      <c r="K21" s="2">
+      <c r="L21" s="2">
         <v>2015</v>
       </c>
-      <c r="L21" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M21" s="2">
+      <c r="M21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N21" s="2">
         <v>-25.7834</v>
       </c>
-      <c r="N21" s="2">
+      <c r="O21" s="2">
         <v>28.281099999999999</v>
       </c>
-      <c r="O21" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P21" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2">
         <v>67891</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>128</v>
-      </c>
       <c r="D22" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>23</v>
+        <v>124</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22" s="2">
+        <v>22</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="7">
         <v>2195</v>
       </c>
-      <c r="H22" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I22" s="2">
+      <c r="I22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J22" s="2">
         <v>900</v>
       </c>
-      <c r="J22" s="2">
+      <c r="K22" s="2">
         <v>450</v>
       </c>
-      <c r="K22" s="2">
+      <c r="L22" s="2">
         <v>2003</v>
       </c>
-      <c r="L22" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="M22" s="2">
+      <c r="M22" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="N22" s="2">
         <v>-26.145600000000002</v>
       </c>
-      <c r="N22" s="2">
+      <c r="O22" s="2">
         <v>27.991099999999999</v>
       </c>
-      <c r="O22" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P22" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2">
         <v>78901</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="D23" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E23" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G23" s="2">
+      <c r="H23" s="7">
         <v>181</v>
       </c>
-      <c r="H23" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I23" s="2">
+      <c r="I23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J23" s="2">
         <v>1600</v>
       </c>
-      <c r="J23" s="2">
+      <c r="K23" s="2">
         <v>1400</v>
       </c>
-      <c r="K23" s="2">
+      <c r="L23" s="2">
         <v>2018</v>
       </c>
-      <c r="L23" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="M23" s="2">
+      <c r="M23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N23" s="2">
         <v>-25.7789</v>
       </c>
-      <c r="N23" s="2">
+      <c r="O23" s="2">
         <v>28.2211</v>
       </c>
-      <c r="O23" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P23" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2">
         <v>89013</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>135</v>
-      </c>
       <c r="D24" s="3" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>23</v>
+        <v>131</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" s="2">
+        <v>22</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="7">
         <v>1684</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="I24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J24" s="2">
+        <v>1800</v>
+      </c>
+      <c r="K24" s="2">
+        <v>900</v>
+      </c>
+      <c r="L24" s="2">
+        <v>2021</v>
+      </c>
+      <c r="M24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I24" s="2">
-        <v>1800</v>
-      </c>
-      <c r="J24" s="2">
-        <v>900</v>
-      </c>
-      <c r="K24" s="2">
-        <v>2021</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M24" s="2">
+      <c r="N24" s="2">
         <v>-25.9876</v>
       </c>
-      <c r="N24" s="2">
+      <c r="O24" s="2">
         <v>28.071100000000001</v>
       </c>
-      <c r="O24" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P24" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>24</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2">
         <v>90123</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="D25" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" s="2">
+      <c r="H25" s="10">
         <v>181</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="I25" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J25" s="11">
+        <v>2500</v>
+      </c>
+      <c r="K25" s="11">
+        <v>2000</v>
+      </c>
+      <c r="L25" s="11">
+        <v>2014</v>
+      </c>
+      <c r="M25" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="I25" s="2">
-        <v>2500</v>
-      </c>
-      <c r="J25" s="2">
-        <v>2000</v>
-      </c>
-      <c r="K25" s="2">
-        <v>2014</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M25" s="2">
+      <c r="N25" s="11">
         <v>-25.7623</v>
       </c>
-      <c r="N25" s="2">
+      <c r="O25" s="11">
         <v>28.241099999999999</v>
       </c>
-      <c r="O25" s="4" t="s">
-        <v>139</v>
+      <c r="P25" s="12" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O5" r:id="rId1" display="https://example.com/property4_1.jpg,https:/example.com/property4_2.jpg" xr:uid="{B8281692-31CA-4AE0-B186-AB70AA9537B0}"/>
-    <hyperlink ref="O6" r:id="rId2" xr:uid="{1DE41EE4-5AB5-4EB0-B645-3C53B65D8A88}"/>
-    <hyperlink ref="O7" r:id="rId3" display="https://example.com/property6_1.jpg,https:/example.com/property6_2.jpg" xr:uid="{04331E63-E250-4258-BF06-C2F3AE057D6D}"/>
-    <hyperlink ref="O8" r:id="rId4" xr:uid="{A32C1ED0-9932-43FE-8DEA-405F41C7283B}"/>
-    <hyperlink ref="O9" r:id="rId5" xr:uid="{CF6314B9-C2F6-43A4-8E56-26075E70E512}"/>
-    <hyperlink ref="O10" r:id="rId6" xr:uid="{5AB96263-7476-436B-AD70-E3CBB9E324FD}"/>
-    <hyperlink ref="O11" r:id="rId7" display="https://example.com/property10_1.jpg,https:/example.com/property10_2.jpg" xr:uid="{DBDA833B-DC78-441D-9AED-C3417FD6C3CE}"/>
-    <hyperlink ref="O12" r:id="rId8" xr:uid="{781C5E49-21B0-458A-A2FF-135C15C95994}"/>
-    <hyperlink ref="O13" r:id="rId9" xr:uid="{C198BE95-B990-46BD-9009-EEA180F19EA6}"/>
-    <hyperlink ref="O14" r:id="rId10" xr:uid="{A2BD020E-629C-415E-AA8C-888D1D257313}"/>
-    <hyperlink ref="O15" r:id="rId11" display="https://example.com/property14_1.jpg,https:/example.com/property14_2.jpg" xr:uid="{9AFA750E-92E2-4AED-AE66-75E87C3BA5E8}"/>
-    <hyperlink ref="O16" r:id="rId12" xr:uid="{3F9F7282-EEFE-42FC-BF97-0AEE4F44B1A0}"/>
-    <hyperlink ref="O17" r:id="rId13" xr:uid="{73515211-81BB-4CF7-82F7-772CB2C8F2B7}"/>
-    <hyperlink ref="O18" r:id="rId14" xr:uid="{4F3722FF-D132-483F-BD0A-603F937F7D92}"/>
-    <hyperlink ref="O19" r:id="rId15" xr:uid="{B9F616BF-7A35-4026-B113-25A77404FDAE}"/>
-    <hyperlink ref="O20" r:id="rId16" xr:uid="{267D9DDF-D051-41C8-973F-6EA54FD77A01}"/>
-    <hyperlink ref="O21" r:id="rId17" xr:uid="{8E827588-6CAE-4FEB-9BD5-DA681B4D44BB}"/>
-    <hyperlink ref="O22" r:id="rId18" xr:uid="{464AE8BC-6AE0-406F-82DD-ADD2541C3EE1}"/>
-    <hyperlink ref="O23" r:id="rId19" xr:uid="{4A3753B6-09AA-465A-8AE9-15DA04B025A0}"/>
-    <hyperlink ref="O24" r:id="rId20" xr:uid="{8591CAD0-0354-40E5-AA40-9122B87242B0}"/>
-    <hyperlink ref="O25" r:id="rId21" xr:uid="{D9930425-BFF7-4DB7-8533-A94CEB9E29CD}"/>
+    <hyperlink ref="P5" r:id="rId1" display="https://example.com/property4_1.jpg,https:/example.com/property4_2.jpg" xr:uid="{B8281692-31CA-4AE0-B186-AB70AA9537B0}"/>
+    <hyperlink ref="P6" r:id="rId2" xr:uid="{1DE41EE4-5AB5-4EB0-B645-3C53B65D8A88}"/>
+    <hyperlink ref="P8" r:id="rId3" xr:uid="{A32C1ED0-9932-43FE-8DEA-405F41C7283B}"/>
+    <hyperlink ref="P10" r:id="rId4" xr:uid="{5AB96263-7476-436B-AD70-E3CBB9E324FD}"/>
+    <hyperlink ref="P11" r:id="rId5" display="https://example.com/property10_1.jpg,https:/example.com/property10_2.jpg" xr:uid="{DBDA833B-DC78-441D-9AED-C3417FD6C3CE}"/>
+    <hyperlink ref="P12" r:id="rId6" xr:uid="{781C5E49-21B0-458A-A2FF-135C15C95994}"/>
+    <hyperlink ref="P14" r:id="rId7" xr:uid="{A2BD020E-629C-415E-AA8C-888D1D257313}"/>
+    <hyperlink ref="P15" r:id="rId8" display="https://example.com/property14_1.jpg,https:/example.com/property14_2.jpg" xr:uid="{9AFA750E-92E2-4AED-AE66-75E87C3BA5E8}"/>
+    <hyperlink ref="P16" r:id="rId9" xr:uid="{3F9F7282-EEFE-42FC-BF97-0AEE4F44B1A0}"/>
+    <hyperlink ref="P17" r:id="rId10" xr:uid="{73515211-81BB-4CF7-82F7-772CB2C8F2B7}"/>
+    <hyperlink ref="P18" r:id="rId11" xr:uid="{4F3722FF-D132-483F-BD0A-603F937F7D92}"/>
+    <hyperlink ref="P19" r:id="rId12" xr:uid="{B9F616BF-7A35-4026-B113-25A77404FDAE}"/>
+    <hyperlink ref="P20" r:id="rId13" xr:uid="{267D9DDF-D051-41C8-973F-6EA54FD77A01}"/>
+    <hyperlink ref="P21" r:id="rId14" xr:uid="{8E827588-6CAE-4FEB-9BD5-DA681B4D44BB}"/>
+    <hyperlink ref="P22" r:id="rId15" xr:uid="{464AE8BC-6AE0-406F-82DD-ADD2541C3EE1}"/>
+    <hyperlink ref="P23" r:id="rId16" xr:uid="{4A3753B6-09AA-465A-8AE9-15DA04B025A0}"/>
+    <hyperlink ref="P24" r:id="rId17" xr:uid="{8591CAD0-0354-40E5-AA40-9122B87242B0}"/>
+    <hyperlink ref="P25" r:id="rId18" xr:uid="{D9930425-BFF7-4DB7-8533-A94CEB9E29CD}"/>
+    <hyperlink ref="P2" r:id="rId19" xr:uid="{2BA9D6FB-5E66-49EC-8149-5E07451A2E66}"/>
+    <hyperlink ref="P7" r:id="rId20" xr:uid="{66BD5155-4E19-4CEF-A190-441B7B38B4D3}"/>
+    <hyperlink ref="P9" r:id="rId21" xr:uid="{2E1D70C1-AE7C-444E-8506-2BE79DA6507F}"/>
+    <hyperlink ref="P13" r:id="rId22" xr:uid="{E7A338FE-44CB-45FB-BD13-75E6A7A2C265}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
+  <tableParts count="1">
+    <tablePart r:id="rId24"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -2089,25 +2712,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -2118,19 +2741,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
         <v>43</v>
-      </c>
-      <c r="E2" t="s">
-        <v>45</v>
       </c>
       <c r="F2">
         <v>50000000</v>
       </c>
       <c r="G2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2141,19 +2764,19 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
         <v>41</v>
       </c>
-      <c r="D3" t="s">
-        <v>43</v>
-      </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F3">
         <v>3500000</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -2164,19 +2787,19 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" t="s">
-        <v>44</v>
-      </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F4">
         <v>45000000</v>
       </c>
       <c r="G4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2202,22 +2825,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2228,16 +2851,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D2">
         <v>55000000</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -2248,16 +2871,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D3">
         <v>3800000</v>
       </c>
       <c r="E3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" t="s">
         <v>58</v>
-      </c>
-      <c r="F3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -2268,16 +2891,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D4">
         <v>47000000</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2302,19 +2925,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2325,13 +2948,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -2342,13 +2965,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -2359,13 +2982,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2393,7 +3016,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -2405,16 +3028,16 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -2422,13 +3045,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2">
         <v>4500000</v>
@@ -2440,7 +3063,7 @@
         <v>8.5</v>
       </c>
       <c r="H2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -2448,13 +3071,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
         <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
       </c>
       <c r="E3">
         <v>1800000</v>
@@ -2466,7 +3089,7 @@
         <v>5</v>
       </c>
       <c r="H3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -2474,13 +3097,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4">
         <v>4200000</v>
@@ -2492,7 +3115,7 @@
         <v>6.5</v>
       </c>
       <c r="H4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement AWS-inspired theme across entire dashboard
- Added comprehensive AWS theme variables (aws-theme.css)
- Created AWS-styled components (AWSComponents.css)
- Updated Properties page with AWS styling (PropertiesAWS.css)
- Implemented AWS modal design (PropertyModalAWS.css)
- Added global AWS styling system (aws-global.css)
- Updated all component imports to use AWS styles
- Maintained all existing functionality while changing only visual theme
- Applied AWS color palette: Orange (#FF9900), Navy (#232F3E), Clean whites/grays
- Implemented AWS-style typography, buttons, cards, and interactions
</commit_message>
<xml_diff>
--- a/property_research_sample.xlsx
+++ b/property_research_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amoge\Digital Estate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E87278A-88C1-4B0A-8E61-92C5882E7966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD00D685-D062-44A2-A8B8-E2E8FE9BE896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8100" yWindow="-15000" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="properties" sheetId="1" r:id="rId1"/>
@@ -1132,7 +1132,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D22670CB-BC3B-4D82-B15C-2A04F0AE5DD4}" name="Table1" displayName="Table1" ref="D1:P25" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="15" tableBorderDxfId="16">
-  <autoFilter ref="D1:P25" xr:uid="{D22670CB-BC3B-4D82-B15C-2A04F0AE5DD4}"/>
+  <autoFilter ref="D1:P25" xr:uid="{D22670CB-BC3B-4D82-B15C-2A04F0AE5DD4}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Sandton"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{999FD1A3-128A-4F56-88BC-FED56F3EA866}" name="street_address" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{E2A59FC4-0C3E-4E3B-B9E0-C2B01872C1B7}" name="suburb" dataDxfId="13"/>
@@ -1462,7 +1468,7 @@
     <col min="13" max="13" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="69.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="80" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -1515,7 +1521,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1565,7 +1571,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1609,7 +1615,7 @@
         <v>28.1891</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1653,7 +1659,7 @@
         <v>28.0411</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1701,7 +1707,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1797,7 +1803,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1893,7 +1899,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1941,7 +1947,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1989,7 +1995,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" ht="27.6" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2085,7 +2091,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2133,7 +2139,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2181,7 +2187,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" ht="27.6" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2229,7 +2235,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2277,7 +2283,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2325,7 +2331,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2373,7 +2379,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -2421,7 +2427,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -2469,7 +2475,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -2517,7 +2523,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" ht="27.6" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -2565,7 +2571,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -2613,7 +2619,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>24</v>
       </c>

</xml_diff>